<commit_message>
Update vending source document item price
</commit_message>
<xml_diff>
--- a/Data/Input/Vending-Items.xlsx
+++ b/Data/Input/Vending-Items.xlsx
@@ -461,7 +461,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,7 +477,7 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>